<commit_message>
debug tables and get Turnigy to run
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/calibration20161009.xlsx
+++ b/myESC-Particle-DEV/saves/calibration20161009.xlsx
@@ -895,10 +895,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>CalArduino!$J$2:$J$30</c:f>
+              <c:f>CalArduino!$J$2:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>11.64</c:v>
                 </c:pt>
@@ -925,10 +925,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>CalArduino!$Q$2:$Q$30</c:f>
+              <c:f>CalArduino!$Q$2:$Q$8</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="29"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>35.26475694444445</c:v>
                 </c:pt>
@@ -963,11 +963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209583336"/>
-        <c:axId val="209585296"/>
+        <c:axId val="112205328"/>
+        <c:axId val="112207680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209583336"/>
+        <c:axId val="112205328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,12 +1080,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209585296"/>
+        <c:crossAx val="112207680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209585296"/>
+        <c:axId val="112207680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1198,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209583336"/>
+        <c:crossAx val="112205328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1479,11 +1479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210758888"/>
-        <c:axId val="210762808"/>
+        <c:axId val="112200232"/>
+        <c:axId val="112200624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210758888"/>
+        <c:axId val="112200232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,12 +1540,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210762808"/>
+        <c:crossAx val="112200624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210762808"/>
+        <c:axId val="112200624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,7 +1602,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210758888"/>
+        <c:crossAx val="112200232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1849,11 +1849,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210760064"/>
-        <c:axId val="210760456"/>
+        <c:axId val="89979760"/>
+        <c:axId val="89980936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210760064"/>
+        <c:axId val="89979760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -1967,12 +1967,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210760456"/>
+        <c:crossAx val="89980936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210760456"/>
+        <c:axId val="89980936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2085,7 +2085,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210760064"/>
+        <c:crossAx val="89979760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2149,6 +2149,341 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CalArduino!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fan, %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CalArduino!$Q$2:$Q$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>35.26475694444445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.58385744234802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55.272108843537424</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.708333333333343</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.164075993091544</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>84.10973084886129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>96.176609848484858</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50.340768277571257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CalArduino!$R$2:$R$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>14.799635701275045</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.345984598459847</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.26475694444445</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45.44183445190157</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49.064009661835762</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.117737003058117</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.030141843971634</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.545068027210888</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="111995664"/>
+        <c:axId val="111992136"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="111995664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111992136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="111992136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="111995664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2174,6 +2509,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2352,11 +2688,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="212114848"/>
-        <c:axId val="212113672"/>
+        <c:axId val="89974664"/>
+        <c:axId val="89977016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="212114848"/>
+        <c:axId val="89974664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,6 +2738,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2468,12 +2805,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212113672"/>
+        <c:crossAx val="89977016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="212113672"/>
+        <c:axId val="89977016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2520,6 +2857,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2586,7 +2924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212114848"/>
+        <c:crossAx val="89974664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2795,6 +3133,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4344,6 +4722,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4923,16 +5817,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>68586</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>384810</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>129546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>80010</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>60966</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>346710</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121926</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4946,6 +5840,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>167646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>6</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5280,9 +6204,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH21" sqref="AH21"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5442,7 +6366,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:N8" si="2">1/G2/0.000001</f>
+        <f t="shared" ref="M2:N9" si="2">1/G2/0.000001</f>
         <v>260.41666666666669</v>
       </c>
       <c r="N2" s="3">
@@ -5450,7 +6374,7 @@
         <v>109.2896174863388</v>
       </c>
       <c r="O2" s="3">
-        <f t="shared" ref="O2:P8" si="3">M2*60/$AB$2</f>
+        <f t="shared" ref="O2:P9" si="3">M2*60/$AB$2</f>
         <v>7812.5000000000009</v>
       </c>
       <c r="P2" s="3">
@@ -5458,7 +6382,7 @@
         <v>3278.688524590164</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:R8" si="4">O2/$AB$7*100</f>
+        <f t="shared" ref="Q2:R9" si="4">O2/$AB$7*100</f>
         <v>35.26475694444445</v>
       </c>
       <c r="R2" s="3">
@@ -5466,7 +6390,7 @@
         <v>14.799635701275045</v>
       </c>
       <c r="S2" s="3">
-        <f t="shared" ref="S2:S8" si="5">P2*$AE$10+$AE$11</f>
+        <f t="shared" ref="S2:S9" si="5">P2*$AE$10+$AE$11</f>
         <v>7656.5024245703744</v>
       </c>
       <c r="T2" s="3">
@@ -5474,7 +6398,7 @@
         <v>87</v>
       </c>
       <c r="U2" s="3">
-        <f t="shared" ref="U2:U8" si="7">S2/$AB$7*100</f>
+        <f t="shared" ref="U2:U9" si="7">S2/$AB$7*100</f>
         <v>34.560601222019052</v>
       </c>
       <c r="V2" s="3">
@@ -6117,6 +7041,85 @@
       <c r="AJ8" s="8"/>
     </row>
     <row r="9" spans="1:38" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="1">
+        <v>78.5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2690</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3920</v>
+      </c>
+      <c r="I9" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" ref="J9" si="13">E9*F9</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" ref="K9" si="14">C9</f>
+        <v>78.5</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" ref="L9" si="15">LN(K9)</f>
+        <v>4.3630986247883632</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" ref="M9" si="16">1/G9/0.000001</f>
+        <v>371.74721189591077</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" ref="N9" si="17">1/H9/0.000001</f>
+        <v>255.10204081632656</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" ref="O9" si="18">M9*60/$AB$2</f>
+        <v>11152.416356877324</v>
+      </c>
+      <c r="P9" s="3">
+        <f t="shared" ref="P9" si="19">N9*60/$AB$2</f>
+        <v>7653.0612244897966</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" ref="Q9" si="20">O9/$AB$7*100</f>
+        <v>50.340768277571257</v>
+      </c>
+      <c r="R9" s="3">
+        <f t="shared" ref="R9" si="21">P9/$AB$7*100</f>
+        <v>34.545068027210888</v>
+      </c>
+      <c r="S9" s="3">
+        <f t="shared" ref="S9" si="22">P9*$AE$10+$AE$11</f>
+        <v>12294.237217310983</v>
+      </c>
+      <c r="T9" s="3">
+        <f t="shared" ref="T9" si="23">K9</f>
+        <v>78.5</v>
+      </c>
+      <c r="U9" s="3">
+        <f t="shared" ref="U9" si="24">S9/$AB$7*100</f>
+        <v>55.494820772584305</v>
+      </c>
+      <c r="V9" s="3">
+        <f t="shared" ref="V9" si="25">$AB$13*LN(C9)+$AB$14</f>
+        <v>5202.5413327160204</v>
+      </c>
+      <c r="W9" s="3">
+        <f t="shared" ref="W9" si="26">D9*D9*$AB$10+D9*$AB$11+$AB$12</f>
+        <v>7681.8354489337862</v>
+      </c>
+      <c r="X9" s="3">
+        <f t="shared" ref="X9" si="27">W9/$AB$7*100</f>
+        <v>34.674951679215013</v>
+      </c>
+      <c r="Y9" s="4">
+        <f t="shared" ref="Y9" si="28">J9</f>
+        <v>0</v>
+      </c>
       <c r="AA9" t="s">
         <v>57</v>
       </c>
@@ -6220,7 +7223,7 @@
         <v>27</v>
       </c>
       <c r="AJ11" s="60">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="AK11" s="61">
         <v>-5</v>
@@ -6275,10 +7278,10 @@
         <v>32</v>
       </c>
       <c r="AJ12" s="60">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="AK12" s="61">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
@@ -6325,7 +7328,7 @@
       <c r="AJ13" s="62"/>
       <c r="AK13" s="63">
         <f>(AK12-AK11)/(AH12-AH11)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:38" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6584,7 +7587,7 @@
       </c>
       <c r="AB22" s="68">
         <f>AJ12</f>
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="AC22" s="30"/>
       <c r="AD22" s="31"/>
@@ -6621,7 +7624,7 @@
       </c>
       <c r="AB23" s="68">
         <f>AJ11</f>
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="AC23" s="30"/>
       <c r="AD23" s="31"/>
@@ -6739,7 +7742,7 @@
       </c>
       <c r="AC26" s="71">
         <f>AK13</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AD26" s="31"/>
     </row>
@@ -6875,9 +7878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ13" sqref="AJ13"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7028,7 +8031,7 @@
         <v>18.954000000000001</v>
       </c>
       <c r="K2" s="1">
-        <f t="shared" ref="K2:K8" si="1">C2</f>
+        <f>C2</f>
         <v>61</v>
       </c>
       <c r="L2" s="1">
@@ -7036,51 +8039,51 @@
         <v>4.1108738641733114</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:N8" si="2">1/G2/0.000001</f>
+        <f>1/G2/0.000001</f>
         <v>262.41235611095965</v>
       </c>
       <c r="N2" s="3">
+        <f>1/H2/0.000001</f>
+        <v>116.07661056297157</v>
+      </c>
+      <c r="O2" s="3">
+        <f t="shared" ref="O2:P9" si="1">M2*60/$AB$2</f>
+        <v>7872.3706833287897</v>
+      </c>
+      <c r="P2" s="3">
+        <f t="shared" si="1"/>
+        <v>3482.2983168891469</v>
+      </c>
+      <c r="Q2" s="3">
+        <f t="shared" ref="Q2:R9" si="2">O2/$AB$7*100</f>
+        <v>35.535006556692458</v>
+      </c>
+      <c r="R2" s="3">
         <f t="shared" si="2"/>
-        <v>116.07661056297157</v>
-      </c>
-      <c r="O2" s="3">
-        <f t="shared" ref="O2:P8" si="3">M2*60/$AB$2</f>
+        <v>15.7187076804024</v>
+      </c>
+      <c r="S2" s="3">
+        <f t="shared" ref="S2:S9" si="3">P2*$AE$10+$AE$11</f>
         <v>7872.3706833287897</v>
       </c>
-      <c r="P2" s="3">
-        <f t="shared" si="3"/>
-        <v>3482.2983168891469</v>
-      </c>
-      <c r="Q2" s="3">
-        <f t="shared" ref="Q2:R8" si="4">O2/$AB$7*100</f>
+      <c r="T2" s="3">
+        <f t="shared" ref="T2:T9" si="4">K2</f>
+        <v>61</v>
+      </c>
+      <c r="U2" s="3">
+        <f t="shared" ref="U2:U9" si="5">S2/$AB$7*100</f>
         <v>35.535006556692458</v>
       </c>
-      <c r="R2" s="3">
-        <f t="shared" si="4"/>
-        <v>15.7187076804024</v>
-      </c>
-      <c r="S2" s="3">
-        <f t="shared" ref="S2:S8" si="5">P2*$AE$10+$AE$11</f>
-        <v>7872.3706833287897</v>
-      </c>
-      <c r="T2" s="3">
-        <f t="shared" ref="T2:T8" si="6">K2</f>
-        <v>61</v>
-      </c>
-      <c r="U2" s="3">
-        <f t="shared" ref="U2:U8" si="7">S2/$AB$7*100</f>
-        <v>35.535006556692458</v>
-      </c>
       <c r="V2" s="3">
-        <f t="shared" ref="V2:V8" si="8">$AB$13*LN(C2)+$AB$14</f>
+        <f>$AB$13*LN(C2)+$AB$14</f>
         <v>7969.848528624163</v>
       </c>
       <c r="W2" s="3">
-        <f t="shared" ref="W2:W8" si="9">D2*D2*$AB$10+D2*$AB$11+$AB$12</f>
+        <f>D2*D2*$AB$10+D2*$AB$11+$AB$12</f>
         <v>3895.0045670565887</v>
       </c>
       <c r="X2" s="3">
-        <f t="shared" ref="X2:X8" si="10">W2/$AB$7*100</f>
+        <f t="shared" ref="X2:X9" si="6">W2/$AB$7*100</f>
         <v>17.581617837408213</v>
       </c>
       <c r="Y2" s="4">
@@ -7131,63 +8134,63 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J7" si="11">E3*F3</f>
+        <f t="shared" ref="J3:J7" si="7">E3*F3</f>
         <v>23.065999999999999</v>
       </c>
       <c r="K3" s="1">
+        <f>C3</f>
+        <v>65</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L9" si="8">LN(K3)</f>
+        <v>4.1743872698956368</v>
+      </c>
+      <c r="M3" s="3">
+        <f>1/G3/0.000001</f>
+        <v>307.90143653592179</v>
+      </c>
+      <c r="N3" s="3">
+        <f>1/H3/0.000001</f>
+        <v>158.98251192368841</v>
+      </c>
+      <c r="O3" s="3">
         <f t="shared" si="1"/>
-        <v>65</v>
-      </c>
-      <c r="L3" s="1">
-        <f t="shared" ref="L3:L8" si="12">LN(K3)</f>
-        <v>4.1743872698956368</v>
-      </c>
-      <c r="M3" s="3">
+        <v>9237.0430960776539</v>
+      </c>
+      <c r="P3" s="3">
+        <f t="shared" si="1"/>
+        <v>4769.4753577106521</v>
+      </c>
+      <c r="Q3" s="3">
         <f t="shared" si="2"/>
-        <v>307.90143653592179</v>
-      </c>
-      <c r="N3" s="3">
+        <v>41.694986197572746</v>
+      </c>
+      <c r="R3" s="3">
         <f t="shared" si="2"/>
-        <v>158.98251192368841</v>
-      </c>
-      <c r="O3" s="3">
+        <v>21.528881822999473</v>
+      </c>
+      <c r="S3" s="3">
         <f t="shared" si="3"/>
         <v>9237.0430960776539</v>
       </c>
-      <c r="P3" s="3">
-        <f t="shared" si="3"/>
-        <v>4769.4753577106521</v>
-      </c>
-      <c r="Q3" s="3">
+      <c r="T3" s="3">
         <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" si="5"/>
         <v>41.694986197572746</v>
       </c>
-      <c r="R3" s="3">
-        <f t="shared" si="4"/>
-        <v>21.528881822999473</v>
-      </c>
-      <c r="S3" s="3">
-        <f t="shared" si="5"/>
-        <v>9237.0430960776539</v>
-      </c>
-      <c r="T3" s="3">
+      <c r="V3" s="3">
+        <f>$AB$13*LN(C3)+$AB$14</f>
+        <v>9305.1024786538328</v>
+      </c>
+      <c r="W3" s="3">
+        <f>D3*D3*$AB$10+D3*$AB$11+$AB$12</f>
+        <v>4863.4075129077619</v>
+      </c>
+      <c r="X3" s="3">
         <f t="shared" si="6"/>
-        <v>65</v>
-      </c>
-      <c r="U3" s="3">
-        <f t="shared" si="7"/>
-        <v>41.694986197572746</v>
-      </c>
-      <c r="V3" s="3">
-        <f t="shared" si="8"/>
-        <v>9305.1024786538328</v>
-      </c>
-      <c r="W3" s="3">
-        <f t="shared" si="9"/>
-        <v>4863.4075129077619</v>
-      </c>
-      <c r="X3" s="3">
-        <f t="shared" si="10"/>
         <v>21.952881134653094</v>
       </c>
       <c r="Y3" s="4">
@@ -7239,63 +8242,63 @@
         <v>7.4</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>44.176200000000001</v>
       </c>
       <c r="K4" s="1">
+        <f>C4</f>
+        <v>77</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="8"/>
+        <v>4.3438054218536841</v>
+      </c>
+      <c r="M4" s="3">
+        <f>1/G4/0.000001</f>
+        <v>431.97925918101981</v>
+      </c>
+      <c r="N4" s="3">
+        <f>1/H4/0.000001</f>
+        <v>276.01435274634281</v>
+      </c>
+      <c r="O4" s="3">
         <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="L4" s="1">
-        <f t="shared" si="12"/>
-        <v>4.3438054218536841</v>
-      </c>
-      <c r="M4" s="3">
+        <v>12959.377775430594</v>
+      </c>
+      <c r="P4" s="3">
+        <f t="shared" si="1"/>
+        <v>8280.4305823902851</v>
+      </c>
+      <c r="Q4" s="3">
         <f t="shared" si="2"/>
-        <v>431.97925918101981</v>
-      </c>
-      <c r="N4" s="3">
+        <v>58.497191347429769</v>
+      </c>
+      <c r="R4" s="3">
         <f t="shared" si="2"/>
-        <v>276.01435274634281</v>
-      </c>
-      <c r="O4" s="3">
+        <v>37.376943601067261</v>
+      </c>
+      <c r="S4" s="3">
         <f t="shared" si="3"/>
         <v>12959.377775430594</v>
       </c>
-      <c r="P4" s="3">
-        <f t="shared" si="3"/>
-        <v>8280.4305823902851</v>
-      </c>
-      <c r="Q4" s="3">
+      <c r="T4" s="3">
         <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="5"/>
         <v>58.497191347429769</v>
       </c>
-      <c r="R4" s="3">
-        <f t="shared" si="4"/>
-        <v>37.376943601067261</v>
-      </c>
-      <c r="S4" s="3">
-        <f t="shared" si="5"/>
-        <v>12959.377775430594</v>
-      </c>
-      <c r="T4" s="3">
+      <c r="V4" s="3">
+        <f>$AB$13*LN(C4)+$AB$14</f>
+        <v>12866.811286991171</v>
+      </c>
+      <c r="W4" s="3">
+        <f>D4*D4*$AB$10+D4*$AB$11+$AB$12</f>
+        <v>8182.7859228288444</v>
+      </c>
+      <c r="X4" s="3">
         <f t="shared" si="6"/>
-        <v>77</v>
-      </c>
-      <c r="U4" s="3">
-        <f t="shared" si="7"/>
-        <v>58.497191347429769</v>
-      </c>
-      <c r="V4" s="3">
-        <f t="shared" si="8"/>
-        <v>12866.811286991171</v>
-      </c>
-      <c r="W4" s="3">
-        <f t="shared" si="9"/>
-        <v>8182.7859228288444</v>
-      </c>
-      <c r="X4" s="3">
-        <f t="shared" si="10"/>
         <v>36.936186457213537</v>
       </c>
       <c r="Y4" s="4">
@@ -7347,63 +8350,63 @@
         <v>9.5</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>77.8596</v>
       </c>
       <c r="K5" s="1">
+        <f>C5</f>
+        <v>88</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="8"/>
+        <v>4.4773368144782069</v>
+      </c>
+      <c r="M5" s="3">
+        <f>1/G5/0.000001</f>
+        <v>528.98552548741941</v>
+      </c>
+      <c r="N5" s="3">
+        <f>1/H5/0.000001</f>
+        <v>367.51194413818456</v>
+      </c>
+      <c r="O5" s="3">
         <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="L5" s="1">
-        <f t="shared" si="12"/>
-        <v>4.4773368144782069</v>
-      </c>
-      <c r="M5" s="3">
+        <v>15869.565764622583</v>
+      </c>
+      <c r="P5" s="3">
+        <f t="shared" si="1"/>
+        <v>11025.358324145536</v>
+      </c>
+      <c r="Q5" s="3">
         <f t="shared" si="2"/>
-        <v>528.98552548741941</v>
-      </c>
-      <c r="N5" s="3">
+        <v>71.633456576421381</v>
+      </c>
+      <c r="R5" s="3">
         <f t="shared" si="2"/>
-        <v>367.51194413818456</v>
-      </c>
-      <c r="O5" s="3">
+        <v>49.76724243537916</v>
+      </c>
+      <c r="S5" s="3">
         <f t="shared" si="3"/>
         <v>15869.565764622583</v>
       </c>
-      <c r="P5" s="3">
-        <f t="shared" si="3"/>
-        <v>11025.358324145536</v>
-      </c>
-      <c r="Q5" s="3">
+      <c r="T5" s="3">
         <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" si="5"/>
         <v>71.633456576421381</v>
       </c>
-      <c r="R5" s="3">
-        <f t="shared" si="4"/>
-        <v>49.76724243537916</v>
-      </c>
-      <c r="S5" s="3">
-        <f t="shared" si="5"/>
-        <v>15869.565764622583</v>
-      </c>
-      <c r="T5" s="3">
+      <c r="V5" s="3">
+        <f>$AB$13*LN(C5)+$AB$14</f>
+        <v>15674.066187387478</v>
+      </c>
+      <c r="W5" s="3">
+        <f>D5*D5*$AB$10+D5*$AB$11+$AB$12</f>
+        <v>10620.908743264476</v>
+      </c>
+      <c r="X5" s="3">
         <f t="shared" si="6"/>
-        <v>88</v>
-      </c>
-      <c r="U5" s="3">
-        <f t="shared" si="7"/>
-        <v>71.633456576421381</v>
-      </c>
-      <c r="V5" s="3">
-        <f t="shared" si="8"/>
-        <v>15674.066187387478</v>
-      </c>
-      <c r="W5" s="3">
-        <f t="shared" si="9"/>
-        <v>10620.908743264476</v>
-      </c>
-      <c r="X5" s="3">
-        <f t="shared" si="10"/>
         <v>47.941601966124367</v>
       </c>
       <c r="Y5" s="4">
@@ -7435,63 +8438,63 @@
         <v>10.5</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>100.6914</v>
       </c>
       <c r="K6" s="1">
+        <f>C6</f>
+        <v>95</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="8"/>
+        <v>4.5538768916005408</v>
+      </c>
+      <c r="M6" s="3">
+        <f>1/G6/0.000001</f>
+        <v>576.18521478815251</v>
+      </c>
+      <c r="N6" s="3">
+        <f>1/H6/0.000001</f>
+        <v>412.03131437989288</v>
+      </c>
+      <c r="O6" s="3">
         <f t="shared" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="L6" s="1">
-        <f t="shared" si="12"/>
-        <v>4.5538768916005408</v>
-      </c>
-      <c r="M6" s="3">
+        <v>17285.556443644575</v>
+      </c>
+      <c r="P6" s="3">
+        <f t="shared" si="1"/>
+        <v>12360.939431396786</v>
+      </c>
+      <c r="Q6" s="3">
         <f t="shared" si="2"/>
-        <v>576.18521478815251</v>
-      </c>
-      <c r="N6" s="3">
+        <v>78.025081169228997</v>
+      </c>
+      <c r="R6" s="3">
         <f t="shared" si="2"/>
-        <v>412.03131437989288</v>
-      </c>
-      <c r="O6" s="3">
+        <v>55.795907155610493</v>
+      </c>
+      <c r="S6" s="3">
         <f t="shared" si="3"/>
         <v>17285.556443644575</v>
       </c>
-      <c r="P6" s="3">
-        <f t="shared" si="3"/>
-        <v>12360.939431396786</v>
-      </c>
-      <c r="Q6" s="3">
+      <c r="T6" s="3">
         <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="5"/>
         <v>78.025081169228997</v>
       </c>
-      <c r="R6" s="3">
-        <f t="shared" si="4"/>
-        <v>55.795907155610493</v>
-      </c>
-      <c r="S6" s="3">
-        <f t="shared" si="5"/>
-        <v>17285.556443644575</v>
-      </c>
-      <c r="T6" s="3">
+      <c r="V6" s="3">
+        <f>$AB$13*LN(C6)+$AB$14</f>
+        <v>17283.182233848318</v>
+      </c>
+      <c r="W6" s="3">
+        <f>D6*D6*$AB$10+D6*$AB$11+$AB$12</f>
+        <v>12464.506405406451</v>
+      </c>
+      <c r="X6" s="3">
         <f t="shared" si="6"/>
-        <v>95</v>
-      </c>
-      <c r="U6" s="3">
-        <f t="shared" si="7"/>
-        <v>78.025081169228997</v>
-      </c>
-      <c r="V6" s="3">
-        <f t="shared" si="8"/>
-        <v>17283.182233848318</v>
-      </c>
-      <c r="W6" s="3">
-        <f t="shared" si="9"/>
-        <v>12464.506405406451</v>
-      </c>
-      <c r="X6" s="3">
-        <f t="shared" si="10"/>
         <v>56.263396968848568</v>
       </c>
       <c r="Y6" s="4">
@@ -7529,63 +8532,63 @@
         <v>12.4</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>155.69400000000002</v>
       </c>
       <c r="K7" s="1">
+        <f>C7</f>
+        <v>105</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="8"/>
+        <v>4.6539603501575231</v>
+      </c>
+      <c r="M7" s="3">
+        <f>1/G7/0.000001</f>
+        <v>647.59544384070819</v>
+      </c>
+      <c r="N7" s="3">
+        <f>1/H7/0.000001</f>
+        <v>479.38638542665387</v>
+      </c>
+      <c r="O7" s="3">
         <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="12"/>
-        <v>4.6539603501575231</v>
-      </c>
-      <c r="M7" s="3">
+        <v>19427.863315221246</v>
+      </c>
+      <c r="P7" s="3">
+        <f t="shared" si="1"/>
+        <v>14381.591562799616</v>
+      </c>
+      <c r="Q7" s="3">
         <f t="shared" si="2"/>
-        <v>647.59544384070819</v>
-      </c>
-      <c r="N7" s="3">
+        <v>87.695216353429245</v>
+      </c>
+      <c r="R7" s="3">
         <f t="shared" si="2"/>
-        <v>479.38638542665387</v>
-      </c>
-      <c r="O7" s="3">
+        <v>64.916906359859382</v>
+      </c>
+      <c r="S7" s="3">
         <f t="shared" si="3"/>
         <v>19427.863315221246</v>
       </c>
-      <c r="P7" s="3">
-        <f t="shared" si="3"/>
-        <v>14381.591562799616</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="T7" s="3">
         <f t="shared" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="5"/>
         <v>87.695216353429245</v>
       </c>
-      <c r="R7" s="3">
-        <f t="shared" si="4"/>
-        <v>64.916906359859382</v>
-      </c>
-      <c r="S7" s="3">
-        <f t="shared" si="5"/>
-        <v>19427.863315221246</v>
-      </c>
-      <c r="T7" s="3">
+      <c r="V7" s="3">
+        <f>$AB$13*LN(C7)+$AB$14</f>
+        <v>19387.255096120716</v>
+      </c>
+      <c r="W7" s="3">
+        <f>D7*D7*$AB$10+D7*$AB$11+$AB$12</f>
+        <v>14500.533861250384</v>
+      </c>
+      <c r="X7" s="3">
         <f t="shared" si="6"/>
-        <v>105</v>
-      </c>
-      <c r="U7" s="3">
-        <f t="shared" si="7"/>
-        <v>87.695216353429245</v>
-      </c>
-      <c r="V7" s="3">
-        <f t="shared" si="8"/>
-        <v>19387.255096120716</v>
-      </c>
-      <c r="W7" s="3">
-        <f t="shared" si="9"/>
-        <v>14500.533861250384</v>
-      </c>
-      <c r="X7" s="3">
-        <f t="shared" si="10"/>
         <v>65.4537986792552</v>
       </c>
       <c r="Y7" s="4">
@@ -7639,59 +8642,59 @@
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1">
+        <f>C8</f>
+        <v>120</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="8"/>
+        <v>4.7874917427820458</v>
+      </c>
+      <c r="M8" s="3">
+        <f>1/G8/0.000001</f>
+        <v>734.29995766057527</v>
+      </c>
+      <c r="N8" s="3">
+        <f>1/H8/0.000001</f>
+        <v>561.16722783389457</v>
+      </c>
+      <c r="O8" s="3">
         <f t="shared" si="1"/>
+        <v>22028.998729817256</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" si="1"/>
+        <v>16835.016835016839</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="2"/>
+        <v>99.436452599869568</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" si="2"/>
+        <v>75.991395435839905</v>
+      </c>
+      <c r="S8" s="3">
+        <f t="shared" si="3"/>
+        <v>22028.99872981726</v>
+      </c>
+      <c r="T8" s="3">
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
-      <c r="L8" s="1">
-        <f t="shared" si="12"/>
-        <v>4.7874917427820458</v>
-      </c>
-      <c r="M8" s="3">
-        <f t="shared" si="2"/>
-        <v>734.29995766057527</v>
-      </c>
-      <c r="N8" s="3">
-        <f t="shared" si="2"/>
-        <v>561.16722783389457</v>
-      </c>
-      <c r="O8" s="3">
-        <f t="shared" si="3"/>
-        <v>22028.998729817256</v>
-      </c>
-      <c r="P8" s="3">
-        <f t="shared" si="3"/>
-        <v>16835.016835016839</v>
-      </c>
-      <c r="Q8" s="3">
-        <f t="shared" si="4"/>
-        <v>99.436452599869568</v>
-      </c>
-      <c r="R8" s="3">
-        <f t="shared" si="4"/>
-        <v>75.991395435839905</v>
-      </c>
-      <c r="S8" s="3">
+      <c r="U8" s="3">
         <f t="shared" si="5"/>
-        <v>22028.99872981726</v>
-      </c>
-      <c r="T8" s="3">
+        <v>99.436452599869583</v>
+      </c>
+      <c r="V8" s="3">
+        <f>$AB$13*LN(C8)+$AB$14</f>
+        <v>22194.509996517023</v>
+      </c>
+      <c r="W8" s="3">
+        <f>D8*D8*$AB$10+D8*$AB$11+$AB$12</f>
+        <v>16835.887969335279</v>
+      </c>
+      <c r="X8" s="3">
         <f t="shared" si="6"/>
-        <v>120</v>
-      </c>
-      <c r="U8" s="3">
-        <f t="shared" si="7"/>
-        <v>99.436452599869583</v>
-      </c>
-      <c r="V8" s="3">
-        <f t="shared" si="8"/>
-        <v>22194.509996517023</v>
-      </c>
-      <c r="W8" s="3">
-        <f t="shared" si="9"/>
-        <v>16835.887969335279</v>
-      </c>
-      <c r="X8" s="3">
-        <f t="shared" si="10"/>
         <v>75.995327639360639</v>
       </c>
       <c r="Y8" s="4">
@@ -7704,6 +8707,50 @@
       <c r="AJ8" s="8"/>
     </row>
     <row r="9" spans="1:38" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K9" s="1">
+        <f>CalArduino!C9</f>
+        <v>78.5</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="8"/>
+        <v>4.3630986247883632</v>
+      </c>
+      <c r="N9" s="1">
+        <f>1/CalArduino!H9/0.000001</f>
+        <v>255.10204081632656</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="1"/>
+        <v>7653.0612244897966</v>
+      </c>
+      <c r="R9" s="1">
+        <f t="shared" si="2"/>
+        <v>34.545068027210888</v>
+      </c>
+      <c r="S9" s="1">
+        <f t="shared" si="3"/>
+        <v>12294.237217310983</v>
+      </c>
+      <c r="T9" s="1">
+        <f t="shared" si="4"/>
+        <v>78.5</v>
+      </c>
+      <c r="U9" s="1">
+        <f t="shared" si="5"/>
+        <v>55.494820772584305</v>
+      </c>
+      <c r="V9" s="1">
+        <f>$AB$13*LN(CalArduino!C9)+$AB$14</f>
+        <v>13272.415822510491</v>
+      </c>
+      <c r="W9" s="3">
+        <f>CalArduino!D9*CalArduino!D9*$AB$10+CalArduino!D9*$AB$11+$AB$12</f>
+        <v>7989.7568741948871</v>
+      </c>
+      <c r="X9" s="3">
+        <f t="shared" si="6"/>
+        <v>36.064874779351925</v>
+      </c>
       <c r="AA9" t="s">
         <v>57</v>
       </c>
@@ -7816,7 +8863,7 @@
         <v>60</v>
       </c>
       <c r="AK11" s="61">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="AL11" t="s">
         <v>60</v>
@@ -7882,7 +8929,7 @@
         <v>115</v>
       </c>
       <c r="AK12" s="61">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
@@ -7905,11 +8952,11 @@
         <v>9237.0430960776539</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" ref="Q13:Q18" si="13">P13/60*$AB$2</f>
+        <f t="shared" ref="Q13:Q18" si="9">P13/60*$AB$2</f>
         <v>307.90143653592179</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" ref="R13:R18" si="14">1/Q13/0.000001</f>
+        <f t="shared" ref="R13:R18" si="10">1/Q13/0.000001</f>
         <v>3247.7925769058029</v>
       </c>
       <c r="S13" s="3"/>
@@ -7940,7 +8987,7 @@
       <c r="AJ13" s="62"/>
       <c r="AK13" s="63">
         <f>(AK12-AK11)/(AH12-AH11)</f>
-        <v>21.212121212121215</v>
+        <v>24.242424242424242</v>
       </c>
     </row>
     <row r="14" spans="1:38" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7963,11 +9010,11 @@
         <v>12959.377775430594</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>431.97925918101981</v>
       </c>
       <c r="R14" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>2314.9259570838622</v>
       </c>
       <c r="S14" s="3"/>
@@ -7995,7 +9042,7 @@
       <c r="AJ14" s="62"/>
       <c r="AK14" s="63">
         <f>AK12-AK13*(AH12-AH11)</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="15" spans="1:38" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8018,11 +9065,11 @@
         <v>15869.565764622583</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>528.98552548741941</v>
       </c>
       <c r="R15" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1890.4108937169444</v>
       </c>
       <c r="S15" s="3"/>
@@ -8065,11 +9112,11 @@
         <v>17285.556443644575</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>576.18521478815251</v>
       </c>
       <c r="R16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1735.553038041201</v>
       </c>
       <c r="S16" s="3"/>
@@ -8107,11 +9154,11 @@
         <v>19427.863315221246</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>647.59544384070819</v>
       </c>
       <c r="R17" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1544.1739275824405</v>
       </c>
       <c r="S17" s="3"/>
@@ -8150,11 +9197,11 @@
         <v>22028.99872981726</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>734.29995766057539</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1361.8412878381814</v>
       </c>
       <c r="S18" s="3"/>
@@ -8408,11 +9455,11 @@
       </c>
       <c r="AB26" s="68">
         <f>AK14</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="AC26" s="71">
         <f>AK13</f>
-        <v>21.212121212121215</v>
+        <v>24.242424242424242</v>
       </c>
       <c r="AD26" s="31"/>
     </row>

</xml_diff>

<commit_message>
drive th to zero at startup
to support hitec esc
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/calibration20161009.xlsx
+++ b/myESC-Particle-DEV/saves/calibration20161009.xlsx
@@ -16,6 +16,7 @@
     <sheet name="CalPhoton" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -963,11 +964,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112205328"/>
-        <c:axId val="112207680"/>
+        <c:axId val="169226952"/>
+        <c:axId val="169227344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112205328"/>
+        <c:axId val="169226952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,12 +1081,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112207680"/>
+        <c:crossAx val="169227344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112207680"/>
+        <c:axId val="169227344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1199,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112205328"/>
+        <c:crossAx val="169226952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1479,11 +1480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="112200232"/>
-        <c:axId val="112200624"/>
+        <c:axId val="169228912"/>
+        <c:axId val="169228128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="112200232"/>
+        <c:axId val="169228912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,12 +1541,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112200624"/>
+        <c:crossAx val="169228128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="112200624"/>
+        <c:axId val="169228128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1602,7 +1603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="112200232"/>
+        <c:crossAx val="169228912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1849,11 +1850,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89979760"/>
-        <c:axId val="89980936"/>
+        <c:axId val="170413816"/>
+        <c:axId val="170413424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89979760"/>
+        <c:axId val="170413816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="60"/>
@@ -1967,12 +1968,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89980936"/>
+        <c:crossAx val="170413424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89980936"/>
+        <c:axId val="170413424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2085,7 +2086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89979760"/>
+        <c:crossAx val="170413816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2297,11 +2298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="111995664"/>
-        <c:axId val="111992136"/>
+        <c:axId val="170414208"/>
+        <c:axId val="170414600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="111995664"/>
+        <c:axId val="170414208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2358,12 +2359,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111992136"/>
+        <c:crossAx val="170414600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="111992136"/>
+        <c:axId val="170414600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,7 +2421,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="111995664"/>
+        <c:crossAx val="170414208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2484,6 +2485,341 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CalArduino!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ng, RPM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CalArduino!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>127.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CalArduino!$O$2:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>7812.5000000000009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9433.962264150945</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12244.897959183674</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000.000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15544.041450777202</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18633.540372670806</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21306.818181818184</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11152.416356877324</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="170412640"/>
+        <c:axId val="170414992"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="170412640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="170414992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="170414992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="170412640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -2509,7 +2845,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2688,11 +3023,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="89974664"/>
-        <c:axId val="89977016"/>
+        <c:axId val="170415776"/>
+        <c:axId val="171017728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="89974664"/>
+        <c:axId val="170415776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2738,7 +3073,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2805,12 +3139,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89977016"/>
+        <c:crossAx val="171017728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89977016"/>
+        <c:axId val="171017728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2857,7 +3191,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2924,7 +3257,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89974664"/>
+        <c:crossAx val="170415776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3173,6 +3506,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5238,6 +5611,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5870,6 +6759,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>45726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>45726</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6206,7 +7125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
+      <selection pane="bottomLeft" activeCell="O1" activeCellId="1" sqref="C1:C9 O1:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6366,7 +7285,7 @@
         <v>4.4659081186545837</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:N9" si="2">1/G2/0.000001</f>
+        <f t="shared" ref="M2:N8" si="2">1/G2/0.000001</f>
         <v>260.41666666666669</v>
       </c>
       <c r="N2" s="3">
@@ -6374,7 +7293,7 @@
         <v>109.2896174863388</v>
       </c>
       <c r="O2" s="3">
-        <f t="shared" ref="O2:P9" si="3">M2*60/$AB$2</f>
+        <f t="shared" ref="O2:P8" si="3">M2*60/$AB$2</f>
         <v>7812.5000000000009</v>
       </c>
       <c r="P2" s="3">
@@ -6382,7 +7301,7 @@
         <v>3278.688524590164</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:R9" si="4">O2/$AB$7*100</f>
+        <f t="shared" ref="Q2:R8" si="4">O2/$AB$7*100</f>
         <v>35.26475694444445</v>
       </c>
       <c r="R2" s="3">
@@ -6390,7 +7309,7 @@
         <v>14.799635701275045</v>
       </c>
       <c r="S2" s="3">
-        <f t="shared" ref="S2:S9" si="5">P2*$AE$10+$AE$11</f>
+        <f t="shared" ref="S2:S8" si="5">P2*$AE$10+$AE$11</f>
         <v>7656.5024245703744</v>
       </c>
       <c r="T2" s="3">
@@ -6398,7 +7317,7 @@
         <v>87</v>
       </c>
       <c r="U2" s="3">
-        <f t="shared" ref="U2:U9" si="7">S2/$AB$7*100</f>
+        <f t="shared" ref="U2:U8" si="7">S2/$AB$7*100</f>
         <v>34.560601222019052</v>
       </c>
       <c r="V2" s="3">
@@ -7057,67 +7976,67 @@
         <v>6.8</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" ref="J9" si="13">E9*F9</f>
+        <f>E9*F9</f>
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" ref="K9" si="14">C9</f>
+        <f>C9</f>
         <v>78.5</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" ref="L9" si="15">LN(K9)</f>
+        <f>LN(K9)</f>
         <v>4.3630986247883632</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" ref="M9" si="16">1/G9/0.000001</f>
+        <f>1/G9/0.000001</f>
         <v>371.74721189591077</v>
       </c>
       <c r="N9" s="3">
-        <f t="shared" ref="N9" si="17">1/H9/0.000001</f>
+        <f>1/H9/0.000001</f>
         <v>255.10204081632656</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" ref="O9" si="18">M9*60/$AB$2</f>
+        <f>M9*60/$AB$2</f>
         <v>11152.416356877324</v>
       </c>
       <c r="P9" s="3">
-        <f t="shared" ref="P9" si="19">N9*60/$AB$2</f>
+        <f>N9*60/$AB$2</f>
         <v>7653.0612244897966</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" ref="Q9" si="20">O9/$AB$7*100</f>
+        <f>O9/$AB$7*100</f>
         <v>50.340768277571257</v>
       </c>
       <c r="R9" s="3">
-        <f t="shared" ref="R9" si="21">P9/$AB$7*100</f>
+        <f>P9/$AB$7*100</f>
         <v>34.545068027210888</v>
       </c>
       <c r="S9" s="3">
-        <f t="shared" ref="S9" si="22">P9*$AE$10+$AE$11</f>
+        <f>P9*$AE$10+$AE$11</f>
         <v>12294.237217310983</v>
       </c>
       <c r="T9" s="3">
-        <f t="shared" ref="T9" si="23">K9</f>
+        <f>K9</f>
         <v>78.5</v>
       </c>
       <c r="U9" s="3">
-        <f t="shared" ref="U9" si="24">S9/$AB$7*100</f>
+        <f>S9/$AB$7*100</f>
         <v>55.494820772584305</v>
       </c>
       <c r="V9" s="3">
-        <f t="shared" ref="V9" si="25">$AB$13*LN(C9)+$AB$14</f>
+        <f>$AB$13*LN(C9)+$AB$14</f>
         <v>5202.5413327160204</v>
       </c>
       <c r="W9" s="3">
-        <f t="shared" ref="W9" si="26">D9*D9*$AB$10+D9*$AB$11+$AB$12</f>
+        <f>D9*D9*$AB$10+D9*$AB$11+$AB$12</f>
         <v>7681.8354489337862</v>
       </c>
       <c r="X9" s="3">
-        <f t="shared" ref="X9" si="27">W9/$AB$7*100</f>
+        <f>W9/$AB$7*100</f>
         <v>34.674951679215013</v>
       </c>
       <c r="Y9" s="4">
-        <f t="shared" ref="Y9" si="28">J9</f>
+        <f>J9</f>
         <v>0</v>
       </c>
       <c r="AA9" t="s">
@@ -8027,11 +8946,11 @@
         <v>2.88</v>
       </c>
       <c r="J2" s="2">
-        <f>E2*F2</f>
+        <f t="shared" ref="J2:J7" si="1">E2*F2</f>
         <v>18.954000000000001</v>
       </c>
       <c r="K2" s="1">
-        <f>C2</f>
+        <f t="shared" ref="K2:K8" si="2">C2</f>
         <v>61</v>
       </c>
       <c r="L2" s="1">
@@ -8039,51 +8958,51 @@
         <v>4.1108738641733114</v>
       </c>
       <c r="M2" s="3">
-        <f>1/G2/0.000001</f>
+        <f t="shared" ref="M2:N8" si="3">1/G2/0.000001</f>
         <v>262.41235611095965</v>
       </c>
       <c r="N2" s="3">
-        <f>1/H2/0.000001</f>
+        <f t="shared" si="3"/>
         <v>116.07661056297157</v>
       </c>
       <c r="O2" s="3">
-        <f t="shared" ref="O2:P9" si="1">M2*60/$AB$2</f>
+        <f t="shared" ref="O2:P9" si="4">M2*60/$AB$2</f>
         <v>7872.3706833287897</v>
       </c>
       <c r="P2" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3482.2983168891469</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:R9" si="2">O2/$AB$7*100</f>
+        <f t="shared" ref="Q2:R9" si="5">O2/$AB$7*100</f>
         <v>35.535006556692458</v>
       </c>
       <c r="R2" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>15.7187076804024</v>
       </c>
       <c r="S2" s="3">
-        <f t="shared" ref="S2:S9" si="3">P2*$AE$10+$AE$11</f>
+        <f t="shared" ref="S2:S9" si="6">P2*$AE$10+$AE$11</f>
         <v>7872.3706833287897</v>
       </c>
       <c r="T2" s="3">
-        <f t="shared" ref="T2:T9" si="4">K2</f>
+        <f t="shared" ref="T2:T9" si="7">K2</f>
         <v>61</v>
       </c>
       <c r="U2" s="3">
-        <f t="shared" ref="U2:U9" si="5">S2/$AB$7*100</f>
+        <f t="shared" ref="U2:U9" si="8">S2/$AB$7*100</f>
         <v>35.535006556692458</v>
       </c>
       <c r="V2" s="3">
-        <f>$AB$13*LN(C2)+$AB$14</f>
+        <f t="shared" ref="V2:V8" si="9">$AB$13*LN(C2)+$AB$14</f>
         <v>7969.848528624163</v>
       </c>
       <c r="W2" s="3">
-        <f>D2*D2*$AB$10+D2*$AB$11+$AB$12</f>
+        <f t="shared" ref="W2:W8" si="10">D2*D2*$AB$10+D2*$AB$11+$AB$12</f>
         <v>3895.0045670565887</v>
       </c>
       <c r="X2" s="3">
-        <f t="shared" ref="X2:X9" si="6">W2/$AB$7*100</f>
+        <f t="shared" ref="X2:X9" si="11">W2/$AB$7*100</f>
         <v>17.581617837408213</v>
       </c>
       <c r="Y2" s="4">
@@ -8134,63 +9053,63 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J7" si="7">E3*F3</f>
+        <f t="shared" si="1"/>
         <v>23.065999999999999</v>
       </c>
       <c r="K3" s="1">
-        <f>C3</f>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L9" si="8">LN(K3)</f>
+        <f t="shared" ref="L3:L9" si="12">LN(K3)</f>
         <v>4.1743872698956368</v>
       </c>
       <c r="M3" s="3">
-        <f>1/G3/0.000001</f>
+        <f t="shared" si="3"/>
         <v>307.90143653592179</v>
       </c>
       <c r="N3" s="3">
-        <f>1/H3/0.000001</f>
+        <f t="shared" si="3"/>
         <v>158.98251192368841</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9237.0430960776539</v>
       </c>
       <c r="P3" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4769.4753577106521</v>
       </c>
       <c r="Q3" s="3">
-        <f t="shared" si="2"/>
-        <v>41.694986197572746</v>
-      </c>
-      <c r="R3" s="3">
-        <f t="shared" si="2"/>
-        <v>21.528881822999473</v>
-      </c>
-      <c r="S3" s="3">
-        <f t="shared" si="3"/>
-        <v>9237.0430960776539</v>
-      </c>
-      <c r="T3" s="3">
-        <f t="shared" si="4"/>
-        <v>65</v>
-      </c>
-      <c r="U3" s="3">
         <f t="shared" si="5"/>
         <v>41.694986197572746</v>
       </c>
+      <c r="R3" s="3">
+        <f t="shared" si="5"/>
+        <v>21.528881822999473</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" si="6"/>
+        <v>9237.0430960776539</v>
+      </c>
+      <c r="T3" s="3">
+        <f t="shared" si="7"/>
+        <v>65</v>
+      </c>
+      <c r="U3" s="3">
+        <f t="shared" si="8"/>
+        <v>41.694986197572746</v>
+      </c>
       <c r="V3" s="3">
-        <f>$AB$13*LN(C3)+$AB$14</f>
+        <f t="shared" si="9"/>
         <v>9305.1024786538328</v>
       </c>
       <c r="W3" s="3">
-        <f>D3*D3*$AB$10+D3*$AB$11+$AB$12</f>
+        <f t="shared" si="10"/>
         <v>4863.4075129077619</v>
       </c>
       <c r="X3" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>21.952881134653094</v>
       </c>
       <c r="Y3" s="4">
@@ -8242,63 +9161,63 @@
         <v>7.4</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>44.176200000000001</v>
       </c>
       <c r="K4" s="1">
-        <f>C4</f>
+        <f t="shared" si="2"/>
         <v>77</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.3438054218536841</v>
       </c>
       <c r="M4" s="3">
-        <f>1/G4/0.000001</f>
+        <f t="shared" si="3"/>
         <v>431.97925918101981</v>
       </c>
       <c r="N4" s="3">
-        <f>1/H4/0.000001</f>
+        <f t="shared" si="3"/>
         <v>276.01435274634281</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12959.377775430594</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>8280.4305823902851</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="2"/>
-        <v>58.497191347429769</v>
-      </c>
-      <c r="R4" s="3">
-        <f t="shared" si="2"/>
-        <v>37.376943601067261</v>
-      </c>
-      <c r="S4" s="3">
-        <f t="shared" si="3"/>
-        <v>12959.377775430594</v>
-      </c>
-      <c r="T4" s="3">
-        <f t="shared" si="4"/>
-        <v>77</v>
-      </c>
-      <c r="U4" s="3">
         <f t="shared" si="5"/>
         <v>58.497191347429769</v>
       </c>
+      <c r="R4" s="3">
+        <f t="shared" si="5"/>
+        <v>37.376943601067261</v>
+      </c>
+      <c r="S4" s="3">
+        <f t="shared" si="6"/>
+        <v>12959.377775430594</v>
+      </c>
+      <c r="T4" s="3">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="U4" s="3">
+        <f t="shared" si="8"/>
+        <v>58.497191347429769</v>
+      </c>
       <c r="V4" s="3">
-        <f>$AB$13*LN(C4)+$AB$14</f>
+        <f t="shared" si="9"/>
         <v>12866.811286991171</v>
       </c>
       <c r="W4" s="3">
-        <f>D4*D4*$AB$10+D4*$AB$11+$AB$12</f>
+        <f t="shared" si="10"/>
         <v>8182.7859228288444</v>
       </c>
       <c r="X4" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>36.936186457213537</v>
       </c>
       <c r="Y4" s="4">
@@ -8350,63 +9269,63 @@
         <v>9.5</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>77.8596</v>
       </c>
       <c r="K5" s="1">
-        <f>C5</f>
+        <f t="shared" si="2"/>
         <v>88</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.4773368144782069</v>
       </c>
       <c r="M5" s="3">
-        <f>1/G5/0.000001</f>
+        <f t="shared" si="3"/>
         <v>528.98552548741941</v>
       </c>
       <c r="N5" s="3">
-        <f>1/H5/0.000001</f>
+        <f t="shared" si="3"/>
         <v>367.51194413818456</v>
       </c>
       <c r="O5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>15869.565764622583</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11025.358324145536</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="2"/>
-        <v>71.633456576421381</v>
-      </c>
-      <c r="R5" s="3">
-        <f t="shared" si="2"/>
-        <v>49.76724243537916</v>
-      </c>
-      <c r="S5" s="3">
-        <f t="shared" si="3"/>
-        <v>15869.565764622583</v>
-      </c>
-      <c r="T5" s="3">
-        <f t="shared" si="4"/>
-        <v>88</v>
-      </c>
-      <c r="U5" s="3">
         <f t="shared" si="5"/>
         <v>71.633456576421381</v>
       </c>
+      <c r="R5" s="3">
+        <f t="shared" si="5"/>
+        <v>49.76724243537916</v>
+      </c>
+      <c r="S5" s="3">
+        <f t="shared" si="6"/>
+        <v>15869.565764622583</v>
+      </c>
+      <c r="T5" s="3">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+      <c r="U5" s="3">
+        <f t="shared" si="8"/>
+        <v>71.633456576421381</v>
+      </c>
       <c r="V5" s="3">
-        <f>$AB$13*LN(C5)+$AB$14</f>
+        <f t="shared" si="9"/>
         <v>15674.066187387478</v>
       </c>
       <c r="W5" s="3">
-        <f>D5*D5*$AB$10+D5*$AB$11+$AB$12</f>
+        <f t="shared" si="10"/>
         <v>10620.908743264476</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>47.941601966124367</v>
       </c>
       <c r="Y5" s="4">
@@ -8438,63 +9357,63 @@
         <v>10.5</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>100.6914</v>
       </c>
       <c r="K6" s="1">
-        <f>C6</f>
+        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.5538768916005408</v>
       </c>
       <c r="M6" s="3">
-        <f>1/G6/0.000001</f>
+        <f t="shared" si="3"/>
         <v>576.18521478815251</v>
       </c>
       <c r="N6" s="3">
-        <f>1/H6/0.000001</f>
+        <f t="shared" si="3"/>
         <v>412.03131437989288</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17285.556443644575</v>
       </c>
       <c r="P6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>12360.939431396786</v>
       </c>
       <c r="Q6" s="3">
-        <f t="shared" si="2"/>
-        <v>78.025081169228997</v>
-      </c>
-      <c r="R6" s="3">
-        <f t="shared" si="2"/>
-        <v>55.795907155610493</v>
-      </c>
-      <c r="S6" s="3">
-        <f t="shared" si="3"/>
-        <v>17285.556443644575</v>
-      </c>
-      <c r="T6" s="3">
-        <f t="shared" si="4"/>
-        <v>95</v>
-      </c>
-      <c r="U6" s="3">
         <f t="shared" si="5"/>
         <v>78.025081169228997</v>
       </c>
+      <c r="R6" s="3">
+        <f t="shared" si="5"/>
+        <v>55.795907155610493</v>
+      </c>
+      <c r="S6" s="3">
+        <f t="shared" si="6"/>
+        <v>17285.556443644575</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" si="8"/>
+        <v>78.025081169228997</v>
+      </c>
       <c r="V6" s="3">
-        <f>$AB$13*LN(C6)+$AB$14</f>
+        <f t="shared" si="9"/>
         <v>17283.182233848318</v>
       </c>
       <c r="W6" s="3">
-        <f>D6*D6*$AB$10+D6*$AB$11+$AB$12</f>
+        <f t="shared" si="10"/>
         <v>12464.506405406451</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>56.263396968848568</v>
       </c>
       <c r="Y6" s="4">
@@ -8532,63 +9451,63 @@
         <v>12.4</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v>155.69400000000002</v>
       </c>
       <c r="K7" s="1">
-        <f>C7</f>
+        <f t="shared" si="2"/>
         <v>105</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.6539603501575231</v>
       </c>
       <c r="M7" s="3">
-        <f>1/G7/0.000001</f>
+        <f t="shared" si="3"/>
         <v>647.59544384070819</v>
       </c>
       <c r="N7" s="3">
-        <f>1/H7/0.000001</f>
+        <f t="shared" si="3"/>
         <v>479.38638542665387</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19427.863315221246</v>
       </c>
       <c r="P7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>14381.591562799616</v>
       </c>
       <c r="Q7" s="3">
-        <f t="shared" si="2"/>
-        <v>87.695216353429245</v>
-      </c>
-      <c r="R7" s="3">
-        <f t="shared" si="2"/>
-        <v>64.916906359859382</v>
-      </c>
-      <c r="S7" s="3">
-        <f t="shared" si="3"/>
-        <v>19427.863315221246</v>
-      </c>
-      <c r="T7" s="3">
-        <f t="shared" si="4"/>
-        <v>105</v>
-      </c>
-      <c r="U7" s="3">
         <f t="shared" si="5"/>
         <v>87.695216353429245</v>
       </c>
+      <c r="R7" s="3">
+        <f t="shared" si="5"/>
+        <v>64.916906359859382</v>
+      </c>
+      <c r="S7" s="3">
+        <f t="shared" si="6"/>
+        <v>19427.863315221246</v>
+      </c>
+      <c r="T7" s="3">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="U7" s="3">
+        <f t="shared" si="8"/>
+        <v>87.695216353429245</v>
+      </c>
       <c r="V7" s="3">
-        <f>$AB$13*LN(C7)+$AB$14</f>
+        <f t="shared" si="9"/>
         <v>19387.255096120716</v>
       </c>
       <c r="W7" s="3">
-        <f>D7*D7*$AB$10+D7*$AB$11+$AB$12</f>
+        <f t="shared" si="10"/>
         <v>14500.533861250384</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>65.4537986792552</v>
       </c>
       <c r="Y7" s="4">
@@ -8642,59 +9561,59 @@
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1">
-        <f>C8</f>
+        <f t="shared" si="2"/>
         <v>120</v>
       </c>
       <c r="L8" s="1">
+        <f t="shared" si="12"/>
+        <v>4.7874917427820458</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="3"/>
+        <v>734.29995766057527</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="3"/>
+        <v>561.16722783389457</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="4"/>
+        <v>22028.998729817256</v>
+      </c>
+      <c r="P8" s="3">
+        <f t="shared" si="4"/>
+        <v>16835.016835016839</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="5"/>
+        <v>99.436452599869568</v>
+      </c>
+      <c r="R8" s="3">
+        <f t="shared" si="5"/>
+        <v>75.991395435839905</v>
+      </c>
+      <c r="S8" s="3">
+        <f t="shared" si="6"/>
+        <v>22028.99872981726</v>
+      </c>
+      <c r="T8" s="3">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+      <c r="U8" s="3">
         <f t="shared" si="8"/>
-        <v>4.7874917427820458</v>
-      </c>
-      <c r="M8" s="3">
-        <f>1/G8/0.000001</f>
-        <v>734.29995766057527</v>
-      </c>
-      <c r="N8" s="3">
-        <f>1/H8/0.000001</f>
-        <v>561.16722783389457</v>
-      </c>
-      <c r="O8" s="3">
-        <f t="shared" si="1"/>
-        <v>22028.998729817256</v>
-      </c>
-      <c r="P8" s="3">
-        <f t="shared" si="1"/>
-        <v>16835.016835016839</v>
-      </c>
-      <c r="Q8" s="3">
-        <f t="shared" si="2"/>
-        <v>99.436452599869568</v>
-      </c>
-      <c r="R8" s="3">
-        <f t="shared" si="2"/>
-        <v>75.991395435839905</v>
-      </c>
-      <c r="S8" s="3">
-        <f t="shared" si="3"/>
-        <v>22028.99872981726</v>
-      </c>
-      <c r="T8" s="3">
-        <f t="shared" si="4"/>
-        <v>120</v>
-      </c>
-      <c r="U8" s="3">
-        <f t="shared" si="5"/>
         <v>99.436452599869583</v>
       </c>
       <c r="V8" s="3">
-        <f>$AB$13*LN(C8)+$AB$14</f>
+        <f t="shared" si="9"/>
         <v>22194.509996517023</v>
       </c>
       <c r="W8" s="3">
-        <f>D8*D8*$AB$10+D8*$AB$11+$AB$12</f>
+        <f t="shared" si="10"/>
         <v>16835.887969335279</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>75.995327639360639</v>
       </c>
       <c r="Y8" s="4">
@@ -8712,7 +9631,7 @@
         <v>78.5</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4.3630986247883632</v>
       </c>
       <c r="N9" s="1">
@@ -8720,23 +9639,23 @@
         <v>255.10204081632656</v>
       </c>
       <c r="P9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>7653.0612244897966</v>
       </c>
       <c r="R9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>34.545068027210888</v>
       </c>
       <c r="S9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>12294.237217310983</v>
       </c>
       <c r="T9" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>78.5</v>
       </c>
       <c r="U9" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>55.494820772584305</v>
       </c>
       <c r="V9" s="1">
@@ -8748,7 +9667,7 @@
         <v>7989.7568741948871</v>
       </c>
       <c r="X9" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>36.064874779351925</v>
       </c>
       <c r="AA9" t="s">
@@ -8952,11 +9871,11 @@
         <v>9237.0430960776539</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" ref="Q13:Q18" si="9">P13/60*$AB$2</f>
+        <f t="shared" ref="Q13:Q18" si="13">P13/60*$AB$2</f>
         <v>307.90143653592179</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" ref="R13:R18" si="10">1/Q13/0.000001</f>
+        <f t="shared" ref="R13:R18" si="14">1/Q13/0.000001</f>
         <v>3247.7925769058029</v>
       </c>
       <c r="S13" s="3"/>
@@ -9010,11 +9929,11 @@
         <v>12959.377775430594</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>431.97925918101981</v>
       </c>
       <c r="R14" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2314.9259570838622</v>
       </c>
       <c r="S14" s="3"/>
@@ -9065,11 +9984,11 @@
         <v>15869.565764622583</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>528.98552548741941</v>
       </c>
       <c r="R15" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1890.4108937169444</v>
       </c>
       <c r="S15" s="3"/>
@@ -9112,11 +10031,11 @@
         <v>17285.556443644575</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>576.18521478815251</v>
       </c>
       <c r="R16" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1735.553038041201</v>
       </c>
       <c r="S16" s="3"/>
@@ -9154,11 +10073,11 @@
         <v>19427.863315221246</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>647.59544384070819</v>
       </c>
       <c r="R17" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1544.1739275824405</v>
       </c>
       <c r="S17" s="3"/>
@@ -9197,11 +10116,11 @@
         <v>22028.99872981726</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>734.29995766057539</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1361.8412878381814</v>
       </c>
       <c r="S18" s="3"/>

</xml_diff>